<commit_message>
Updated test data to fail one testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel.xlsx
+++ b/src/test/resources/Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TestIntellect\WorkSpace\Raja_WorkSpace\BPTravel_WebAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DA2E58-25F1-4408-9DD7-A8AD0275ED43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5536B9-8170-43EA-B4EB-0EBBCEADCC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{574BCFC8-1EE5-4E77-A5E0-93F5254A47EC}"/>
   </bookViews>
@@ -130,7 +130,7 @@
     <t>UserName=Shivya#Password=Shivya#expectedTitle=BP Travel - Search</t>
   </si>
   <si>
-    <t>UserName=admin#Password=bala#expectedTitle=Please enter a valid user name and password</t>
+    <t>UserName=admin#Password=bala#expectedTitle=Please enter a valid user name and password Bala</t>
   </si>
 </sst>
 </file>

</xml_diff>